<commit_message>
remove duplicate internet variables 24/32
</commit_message>
<xml_diff>
--- a/Matt/Identify One Hotted Categorical.xlsx
+++ b/Matt/Identify One Hotted Categorical.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25306"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25317"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-60" yWindow="0" windowWidth="38160" windowHeight="16280" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="86">
   <si>
     <t>papglb_friend 1</t>
   </si>
@@ -91,6 +91,192 @@
   </si>
   <si>
     <t>3 - papglb_status</t>
+  </si>
+  <si>
+    <t>'AGE_DIFFERENCE',</t>
+  </si>
+  <si>
+    <t>'CHILDREN_IN_HH',</t>
+  </si>
+  <si>
+    <t>'DISTANCEMOVED_10MI',</t>
+  </si>
+  <si>
+    <t>'GENDER_ATTRACTION',</t>
+  </si>
+  <si>
+    <t>'HHINC',</t>
+  </si>
+  <si>
+    <t>'HOW_LONG_AGO_FIRST_COHAB',</t>
+  </si>
+  <si>
+    <t>'HOW_LONG_AGO_FIRST_MET',</t>
+  </si>
+  <si>
+    <t>'HOW_LONG_AGO_FIRST_ROMANTIC',</t>
+  </si>
+  <si>
+    <t>'HOW_LONG_RELATIONSHIP',</t>
+  </si>
+  <si>
+    <t>'PARTNER_MOM_YRSED',</t>
+  </si>
+  <si>
+    <t>'PARTNER_YRSED',</t>
+  </si>
+  <si>
+    <t>'PPAGECAT',</t>
+  </si>
+  <si>
+    <t>'PPHOUSE',</t>
+  </si>
+  <si>
+    <t>'PPHOUSEHOLDSIZE',</t>
+  </si>
+  <si>
+    <t>'Q21A',</t>
+  </si>
+  <si>
+    <t>'Q21B',</t>
+  </si>
+  <si>
+    <t>'Q21C',</t>
+  </si>
+  <si>
+    <t>'Q9',</t>
+  </si>
+  <si>
+    <t>'RELATIONSHIP_QUALITY',</t>
+  </si>
+  <si>
+    <t>'RESPONDENT_MOM_YRSED',</t>
+  </si>
+  <si>
+    <t>'RESPONDENT_YRSED',</t>
+  </si>
+  <si>
+    <t>'ZPFORBORN_CAT',</t>
+  </si>
+  <si>
+    <t>'ZPNHBLACK_CAT',</t>
+  </si>
+  <si>
+    <t>'ZPNHWHITE_CAT']</t>
+  </si>
+  <si>
+    <t>CORESIDENT',</t>
+  </si>
+  <si>
+    <t>'GLBSTATUS',</t>
+  </si>
+  <si>
+    <t>'MARRIED',</t>
+  </si>
+  <si>
+    <t>'MET_THROUGH_AS_COWORKERS',</t>
+  </si>
+  <si>
+    <t>'MET_THROUGH_AS_NEIGHBORS',</t>
+  </si>
+  <si>
+    <t>'MET_THROUGH_FAMILY',</t>
+  </si>
+  <si>
+    <t>'MET_THROUGH_FRIENDS',</t>
+  </si>
+  <si>
+    <t>'PPHHHEAD',</t>
+  </si>
+  <si>
+    <t>'PPMSACAT',</t>
+  </si>
+  <si>
+    <t>'PPNET',</t>
+  </si>
+  <si>
+    <t>'Q31_1', #refused is -1</t>
+  </si>
+  <si>
+    <t>'Q31_2',#refused is -1</t>
+  </si>
+  <si>
+    <t>'Q31_3',#refused is -1</t>
+  </si>
+  <si>
+    <t>'Q31_4',#refused is -1</t>
+  </si>
+  <si>
+    <t>'Q31_5',#refused is -1</t>
+  </si>
+  <si>
+    <t>'Q31_6',#refused is -1</t>
+  </si>
+  <si>
+    <t>'Q31_7',#refused is -1</t>
+  </si>
+  <si>
+    <t>'Q31_8',#refused is -1</t>
+  </si>
+  <si>
+    <t>'SAME_SEX_COUPLE',</t>
+  </si>
+  <si>
+    <t>'US_RAISED',</t>
+  </si>
+  <si>
+    <t>'ZPRURAL_CAT',</t>
+  </si>
+  <si>
+    <t>'PARENTAL_APPROVAL',</t>
+  </si>
+  <si>
+    <t>'Q33_1',  #refused is -1</t>
+  </si>
+  <si>
+    <t>'Q33_2',#refused is -1</t>
+  </si>
+  <si>
+    <t>'Q33_3', #refused is -1</t>
+  </si>
+  <si>
+    <t>'Q33_4', #refused is -1</t>
+  </si>
+  <si>
+    <t>'Q33_5', #refused is -1</t>
+  </si>
+  <si>
+    <t>'Q33_6', #refused is -1</t>
+  </si>
+  <si>
+    <t>'Q33_7',#refused is -1</t>
+  </si>
+  <si>
+    <t>'EITHER_INTERNET_ADJUSTED</t>
+  </si>
+  <si>
+    <t>PAPEVANGELICAL', #change to 0/1 from 1/2, no refused</t>
+  </si>
+  <si>
+    <t>'Q13A', #change to 0/1 from 1/2, refused is -1</t>
+  </si>
+  <si>
+    <t>'Q28', #change to 0/1 from 1/2, refused is -1</t>
+  </si>
+  <si>
+    <t>'Q8A'</t>
+  </si>
+  <si>
+    <t>Q7A'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Q27', </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Q26', </t>
+  </si>
+  <si>
+    <t>Q25',</t>
   </si>
 </sst>
 </file>
@@ -139,7 +325,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="61">
+  <cellStyleXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -201,11 +387,22 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
-  <cellStyles count="61">
+  <cellStyles count="71">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -236,6 +433,11 @@
     <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -266,6 +468,11 @@
     <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -595,10 +802,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F76"/>
+  <dimension ref="A1:F138"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:F12"/>
+    <sheetView tabSelected="1" topLeftCell="A103" workbookViewId="0">
+      <selection activeCell="A119" sqref="A119:A138"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1022,6 +1229,316 @@
         <v>3</v>
       </c>
     </row>
+    <row r="77" spans="1:1">
+      <c r="A77" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1">
+      <c r="A78" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1">
+      <c r="A79" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1">
+      <c r="A80" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1">
+      <c r="A81" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1">
+      <c r="A82" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1">
+      <c r="A83" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1">
+      <c r="A84" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1">
+      <c r="A85" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1">
+      <c r="A86" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1">
+      <c r="A87" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1">
+      <c r="A88" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1">
+      <c r="A89" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1">
+      <c r="A90" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1">
+      <c r="A91" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1">
+      <c r="A92" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1">
+      <c r="A93" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1">
+      <c r="A94" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1">
+      <c r="A95" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1">
+      <c r="A96" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1">
+      <c r="A97" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1">
+      <c r="A98" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1">
+      <c r="A99" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="100" spans="1:1">
+      <c r="A100" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="101" spans="1:1">
+      <c r="A101" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="102" spans="1:1">
+      <c r="A102" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="103" spans="1:1">
+      <c r="A103" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="104" spans="1:1">
+      <c r="A104" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="105" spans="1:1">
+      <c r="A105" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="106" spans="1:1">
+      <c r="A106" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="107" spans="1:1">
+      <c r="A107" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="108" spans="1:1">
+      <c r="A108" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="109" spans="1:1">
+      <c r="A109" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="110" spans="1:1">
+      <c r="A110" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="111" spans="1:1">
+      <c r="A111" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="112" spans="1:1">
+      <c r="A112" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="113" spans="1:1">
+      <c r="A113" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="114" spans="1:1">
+      <c r="A114" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="115" spans="1:1">
+      <c r="A115" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="116" spans="1:1">
+      <c r="A116" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="117" spans="1:1">
+      <c r="A117" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="118" spans="1:1">
+      <c r="A118" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="119" spans="1:1">
+      <c r="A119" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="120" spans="1:1">
+      <c r="A120" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="121" spans="1:1">
+      <c r="A121" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="122" spans="1:1">
+      <c r="A122" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="123" spans="1:1">
+      <c r="A123" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="124" spans="1:1">
+      <c r="A124" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="125" spans="1:1">
+      <c r="A125" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="126" spans="1:1">
+      <c r="A126" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="127" spans="1:1">
+      <c r="A127" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="128" spans="1:1">
+      <c r="A128" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="129" spans="1:1">
+      <c r="A129" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="130" spans="1:1">
+      <c r="A130" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="131" spans="1:1">
+      <c r="A131" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="132" spans="1:1">
+      <c r="A132" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="133" spans="1:1">
+      <c r="A133" s="1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="134" spans="1:1">
+      <c r="A134" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="135" spans="1:1">
+      <c r="A135" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="136" spans="1:1">
+      <c r="A136" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="137" spans="1:1">
+      <c r="A137" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="138" spans="1:1">
+      <c r="A138" t="s">
+        <v>81</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>